<commit_message>
Update and Cost Analyses
Auditing of old design and updating for JLCPCB-assisted assembly and manufacturing
</commit_message>
<xml_diff>
--- a/hardware/BOM_JLC.xlsx
+++ b/hardware/BOM_JLC.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cflee\Documents\GitHub\FROST\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D81258-0916-4993-8DEA-264D45C3DB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9ECA3A-A628-4178-BE59-F34C9A47C504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15645" yWindow="0" windowWidth="13260" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15315" yWindow="0" windowWidth="13590" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -813,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F1:F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H38" sqref="E1:H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,7 +838,7 @@
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>79</v>
       </c>
@@ -841,7 +852,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -854,8 +865,12 @@
       <c r="D2" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <f t="shared" ref="I2:I37" si="0">$E2*G2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>36</v>
       </c>
@@ -868,8 +883,12 @@
       <c r="D3" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
@@ -882,8 +901,12 @@
       <c r="D4" s="4" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -896,8 +919,12 @@
       <c r="D5" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
@@ -910,8 +937,12 @@
       <c r="D6" s="4" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>150</v>
       </c>
@@ -924,8 +955,12 @@
       <c r="D7" s="4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
@@ -938,8 +973,12 @@
       <c r="D8" s="4" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
@@ -952,8 +991,12 @@
       <c r="D9" s="4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>12</v>
       </c>
@@ -966,8 +1009,12 @@
       <c r="D10" s="4" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
@@ -980,8 +1027,12 @@
       <c r="D11" s="4" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>17</v>
       </c>
@@ -994,8 +1045,12 @@
       <c r="D12" s="4" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>37</v>
       </c>
@@ -1008,8 +1063,12 @@
       <c r="D13" s="4" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>22</v>
       </c>
@@ -1022,8 +1081,12 @@
       <c r="D14" s="4" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>20</v>
       </c>
@@ -1036,8 +1099,12 @@
       <c r="D15" s="4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>23</v>
       </c>
@@ -1050,8 +1117,12 @@
       <c r="D16" s="4" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>620</v>
       </c>
@@ -1064,8 +1135,12 @@
       <c r="D17" s="4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>8</v>
       </c>
@@ -1078,8 +1153,12 @@
       <c r="D18" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>100</v>
       </c>
@@ -1092,8 +1171,12 @@
       <c r="D19" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>29</v>
       </c>
@@ -1106,8 +1189,12 @@
       <c r="D20" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>32</v>
       </c>
@@ -1120,8 +1207,12 @@
       <c r="D21" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>39</v>
       </c>
@@ -1134,8 +1225,12 @@
       <c r="D22" s="4" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>30</v>
       </c>
@@ -1148,8 +1243,12 @@
       <c r="D23" s="4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>47</v>
       </c>
@@ -1162,8 +1261,12 @@
       <c r="D24" s="4" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>48</v>
       </c>
@@ -1176,8 +1279,12 @@
       <c r="D25" s="4" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>46</v>
       </c>
@@ -1190,8 +1297,12 @@
       <c r="D26" s="4" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>65</v>
       </c>
@@ -1204,8 +1315,12 @@
       <c r="D27" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>51</v>
       </c>
@@ -1218,8 +1333,12 @@
       <c r="D28" s="4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>61</v>
       </c>
@@ -1232,8 +1351,12 @@
       <c r="D29" s="4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>54</v>
       </c>
@@ -1246,8 +1369,12 @@
       <c r="D30" s="4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>57</v>
       </c>
@@ -1260,8 +1387,12 @@
       <c r="D31" s="4" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>71</v>
       </c>
@@ -1274,8 +1405,12 @@
       <c r="D32" s="4" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>62</v>
       </c>
@@ -1288,8 +1423,12 @@
       <c r="D33" s="4" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>62</v>
       </c>
@@ -1302,8 +1441,12 @@
       <c r="D34" s="4" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>76</v>
       </c>
@@ -1316,8 +1459,12 @@
       <c r="D35" s="4" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>62</v>
       </c>
@@ -1330,8 +1477,12 @@
       <c r="D36" s="4" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
         <v>74</v>
       </c>
@@ -1343,6 +1494,16 @@
       </c>
       <c r="D37" s="5" t="s">
         <v>113</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <f>SUM(I2:I37)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>